<commit_message>
It's getting messier boi
</commit_message>
<xml_diff>
--- a/data/ans.1.xlsx
+++ b/data/ans.1.xlsx
@@ -256,7 +256,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -314,13 +314,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1407,7 +1413,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="5" width="11.6719" style="1" customWidth="1"/>
     <col min="6" max="6" width="6.67188" style="1" customWidth="1"/>
@@ -1485,25 +1491,31 @@
       <c r="B4" s="18">
         <v>1</v>
       </c>
-      <c r="C4" s="18">
-        <v>5825</v>
+      <c r="C4" s="19">
+        <v>5785</v>
       </c>
       <c r="D4" s="18">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E4" s="18">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="19">
+      <c r="G4" s="20">
         <v>0</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="20">
         <v>1</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
+      <c r="I4" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J4" s="20">
+        <v>166</v>
+      </c>
+      <c r="K4" s="20">
+        <v>351</v>
+      </c>
     </row>
     <row r="5" ht="16" customHeight="1">
       <c r="A5" s="18">
@@ -1512,23 +1524,31 @@
       <c r="B5" s="18">
         <v>25</v>
       </c>
-      <c r="C5" s="18">
-        <v>5825</v>
+      <c r="C5" s="19">
+        <v>5785</v>
       </c>
       <c r="D5" s="18">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E5" s="18">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="F5" s="5"/>
-      <c r="G5" s="19">
+      <c r="G5" s="20">
         <v>1</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
+      <c r="H5" s="20">
+        <v>2</v>
+      </c>
+      <c r="I5" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J5" s="20">
+        <v>150</v>
+      </c>
+      <c r="K5" s="20">
+        <v>339</v>
+      </c>
     </row>
     <row r="6" ht="16" customHeight="1">
       <c r="A6" s="18">
@@ -1537,23 +1557,31 @@
       <c r="B6" s="18">
         <v>24</v>
       </c>
-      <c r="C6" s="18">
-        <v>5825</v>
+      <c r="C6" s="19">
+        <v>5785</v>
       </c>
       <c r="D6" s="18">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E6" s="18">
-        <v>303</v>
+        <v>309</v>
       </c>
       <c r="F6" s="5"/>
-      <c r="G6" s="19">
+      <c r="G6" s="20">
         <v>2</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="H6" s="20">
+        <v>3</v>
+      </c>
+      <c r="I6" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J6" s="20">
+        <v>134</v>
+      </c>
+      <c r="K6" s="20">
+        <v>327</v>
+      </c>
     </row>
     <row r="7" ht="16" customHeight="1">
       <c r="A7" s="18">
@@ -1562,23 +1590,31 @@
       <c r="B7" s="18">
         <v>23</v>
       </c>
-      <c r="C7" s="18">
-        <v>5825</v>
+      <c r="C7" s="19">
+        <v>5785</v>
       </c>
       <c r="D7" s="18">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E7" s="18">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="19">
+      <c r="G7" s="20">
         <v>3</v>
       </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
+      <c r="H7" s="20">
+        <v>4</v>
+      </c>
+      <c r="I7" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J7" s="20">
+        <v>124</v>
+      </c>
+      <c r="K7" s="20">
+        <v>313</v>
+      </c>
     </row>
     <row r="8" ht="16" customHeight="1">
       <c r="A8" s="18">
@@ -1587,23 +1623,31 @@
       <c r="B8" s="18">
         <v>23</v>
       </c>
-      <c r="C8" s="18">
-        <v>5825</v>
+      <c r="C8" s="19">
+        <v>5785</v>
       </c>
       <c r="D8" s="18">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E8" s="18">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="F8" s="5"/>
-      <c r="G8" s="19">
+      <c r="G8" s="20">
         <v>4</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
+      <c r="H8" s="20">
+        <v>4</v>
+      </c>
+      <c r="I8" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J8" s="20">
+        <v>114</v>
+      </c>
+      <c r="K8" s="20">
+        <v>303</v>
+      </c>
     </row>
     <row r="9" ht="16" customHeight="1">
       <c r="A9" s="18">
@@ -1612,23 +1656,31 @@
       <c r="B9" s="18">
         <v>22</v>
       </c>
-      <c r="C9" s="18">
-        <v>5825</v>
+      <c r="C9" s="19">
+        <v>5785</v>
       </c>
       <c r="D9" s="18">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E9" s="18">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="F9" s="5"/>
-      <c r="G9" s="19">
+      <c r="G9" s="20">
         <v>5</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
+      <c r="H9" s="20">
+        <v>5</v>
+      </c>
+      <c r="I9" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J9" s="20">
+        <v>104</v>
+      </c>
+      <c r="K9" s="20">
+        <v>289</v>
+      </c>
     </row>
     <row r="10" ht="16" customHeight="1">
       <c r="A10" s="18">
@@ -1637,23 +1689,31 @@
       <c r="B10" s="18">
         <v>9</v>
       </c>
-      <c r="C10" s="18">
-        <v>5825</v>
+      <c r="C10" s="19">
+        <v>5785</v>
       </c>
       <c r="D10" s="18">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E10" s="18">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="F10" s="5"/>
-      <c r="G10" s="19">
+      <c r="G10" s="20">
         <v>6</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
+      <c r="H10" s="20">
+        <v>13</v>
+      </c>
+      <c r="I10" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J10" s="20">
+        <v>88</v>
+      </c>
+      <c r="K10" s="20">
+        <v>277</v>
+      </c>
     </row>
     <row r="11" ht="16" customHeight="1">
       <c r="A11" s="18">
@@ -1662,23 +1722,31 @@
       <c r="B11" s="18">
         <v>9</v>
       </c>
-      <c r="C11" s="18">
-        <v>5825</v>
+      <c r="C11" s="19">
+        <v>5785</v>
       </c>
       <c r="D11" s="18">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E11" s="18">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="F11" s="5"/>
-      <c r="G11" s="19">
+      <c r="G11" s="20">
         <v>7</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
+      <c r="H11" s="20">
+        <v>13</v>
+      </c>
+      <c r="I11" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J11" s="20">
+        <v>78</v>
+      </c>
+      <c r="K11" s="20">
+        <v>267</v>
+      </c>
     </row>
     <row r="12" ht="16" customHeight="1">
       <c r="A12" s="18">
@@ -1687,23 +1755,31 @@
       <c r="B12" s="18">
         <v>15</v>
       </c>
-      <c r="C12" s="18">
-        <v>4185</v>
+      <c r="C12" s="19">
+        <v>4145</v>
       </c>
       <c r="D12" s="18">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E12" s="18">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="F12" s="5"/>
-      <c r="G12" s="19">
+      <c r="G12" s="20">
         <v>8</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
+      <c r="H12" s="20">
+        <v>22</v>
+      </c>
+      <c r="I12" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J12" s="20">
+        <v>68</v>
+      </c>
+      <c r="K12" s="20">
+        <v>253</v>
+      </c>
     </row>
     <row r="13" ht="16" customHeight="1">
       <c r="A13" s="18">
@@ -1712,23 +1788,31 @@
       <c r="B13" s="18">
         <v>13</v>
       </c>
-      <c r="C13" s="18">
-        <v>4185</v>
+      <c r="C13" s="19">
+        <v>4145</v>
       </c>
       <c r="D13" s="18">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E13" s="18">
-        <v>217</v>
+        <v>223</v>
       </c>
       <c r="F13" s="5"/>
-      <c r="G13" s="19">
+      <c r="G13" s="20">
         <v>9</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
+      <c r="H13" s="20">
+        <v>30</v>
+      </c>
+      <c r="I13" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J13" s="20">
+        <v>52</v>
+      </c>
+      <c r="K13" s="20">
+        <v>241</v>
+      </c>
     </row>
     <row r="14" ht="16" customHeight="1">
       <c r="A14" s="18">
@@ -1737,23 +1821,31 @@
       <c r="B14" s="18">
         <v>12</v>
       </c>
-      <c r="C14" s="18">
-        <v>4185</v>
+      <c r="C14" s="19">
+        <v>4145</v>
       </c>
       <c r="D14" s="18">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E14" s="18">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" s="19">
+      <c r="G14" s="20">
         <v>10</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="20"/>
+      <c r="H14" s="20">
+        <v>39</v>
+      </c>
+      <c r="I14" s="21">
+        <v>5660</v>
+      </c>
+      <c r="J14" s="20">
+        <v>36</v>
+      </c>
+      <c r="K14" s="20">
+        <v>229</v>
+      </c>
     </row>
     <row r="15" ht="16" customHeight="1">
       <c r="A15" s="18">
@@ -1762,23 +1854,31 @@
       <c r="B15" s="18">
         <v>12</v>
       </c>
-      <c r="C15" s="18">
-        <v>5185</v>
+      <c r="C15" s="19">
+        <v>5145</v>
       </c>
       <c r="D15" s="18">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E15" s="18">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="F15" s="5"/>
-      <c r="G15" s="19">
+      <c r="G15" s="20">
         <v>11</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
+      <c r="H15" s="20">
+        <v>39</v>
+      </c>
+      <c r="I15" s="21">
+        <v>3290</v>
+      </c>
+      <c r="J15" s="20">
+        <v>247</v>
+      </c>
+      <c r="K15" s="20">
+        <v>227</v>
+      </c>
     </row>
     <row r="16" ht="16" customHeight="1">
       <c r="A16" s="18">
@@ -1787,23 +1887,31 @@
       <c r="B16" s="18">
         <v>12</v>
       </c>
-      <c r="C16" s="18">
-        <v>6185</v>
+      <c r="C16" s="19">
+        <v>6145</v>
       </c>
       <c r="D16" s="18">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E16" s="18">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="F16" s="5"/>
-      <c r="G16" s="19">
+      <c r="G16" s="20">
         <v>12</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
+      <c r="H16" s="20">
+        <v>30</v>
+      </c>
+      <c r="I16" s="21">
+        <v>3290</v>
+      </c>
+      <c r="J16" s="20">
+        <v>231</v>
+      </c>
+      <c r="K16" s="20">
+        <v>215</v>
+      </c>
     </row>
     <row r="17" ht="16" customHeight="1">
       <c r="A17" s="18">
@@ -1812,23 +1920,31 @@
       <c r="B17" s="18">
         <v>12</v>
       </c>
-      <c r="C17" s="18">
-        <v>7185</v>
+      <c r="C17" s="19">
+        <v>7145</v>
       </c>
       <c r="D17" s="18">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E17" s="18">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="F17" s="5"/>
-      <c r="G17" s="19">
+      <c r="G17" s="20">
         <v>13</v>
       </c>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+      <c r="H17" s="20">
+        <v>30</v>
+      </c>
+      <c r="I17" s="21">
+        <v>4290</v>
+      </c>
+      <c r="J17" s="20">
+        <v>216</v>
+      </c>
+      <c r="K17" s="20">
+        <v>194</v>
+      </c>
     </row>
     <row r="18" ht="16" customHeight="1">
       <c r="A18" s="18">
@@ -1837,23 +1953,31 @@
       <c r="B18" s="18">
         <v>12</v>
       </c>
-      <c r="C18" s="18">
-        <v>8185</v>
+      <c r="C18" s="19">
+        <v>8145</v>
       </c>
       <c r="D18" s="18">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E18" s="18">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="F18" s="5"/>
-      <c r="G18" s="19">
+      <c r="G18" s="20">
         <v>14</v>
       </c>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
+      <c r="H18" s="20">
+        <v>30</v>
+      </c>
+      <c r="I18" s="21">
+        <v>5290</v>
+      </c>
+      <c r="J18" s="20">
+        <v>192</v>
+      </c>
+      <c r="K18" s="20">
+        <v>176</v>
+      </c>
     </row>
     <row r="19" ht="16" customHeight="1">
       <c r="A19" s="18">
@@ -1862,23 +1986,31 @@
       <c r="B19" s="18">
         <v>12</v>
       </c>
-      <c r="C19" s="18">
-        <v>9185</v>
+      <c r="C19" s="19">
+        <v>9145</v>
       </c>
       <c r="D19" s="18">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E19" s="18">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="F19" s="5"/>
-      <c r="G19" s="19">
+      <c r="G19" s="20">
         <v>15</v>
       </c>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
+      <c r="H19" s="20">
+        <v>30</v>
+      </c>
+      <c r="I19" s="21">
+        <v>6290</v>
+      </c>
+      <c r="J19" s="20">
+        <v>168</v>
+      </c>
+      <c r="K19" s="20">
+        <v>158</v>
+      </c>
     </row>
     <row r="20" ht="16" customHeight="1">
       <c r="A20" s="18">
@@ -1887,23 +2019,31 @@
       <c r="B20" s="18">
         <v>12</v>
       </c>
-      <c r="C20" s="18">
-        <v>10185</v>
+      <c r="C20" s="19">
+        <v>10145</v>
       </c>
       <c r="D20" s="18">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E20" s="18">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="F20" s="5"/>
-      <c r="G20" s="19">
+      <c r="G20" s="20">
         <v>16</v>
       </c>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="H20" s="20">
+        <v>30</v>
+      </c>
+      <c r="I20" s="21">
+        <v>7290</v>
+      </c>
+      <c r="J20" s="20">
+        <v>144</v>
+      </c>
+      <c r="K20" s="20">
+        <v>140</v>
+      </c>
     </row>
     <row r="21" ht="16" customHeight="1">
       <c r="A21" s="18">
@@ -1912,23 +2052,31 @@
       <c r="B21" s="18">
         <v>12</v>
       </c>
-      <c r="C21" s="18">
-        <v>11185</v>
+      <c r="C21" s="19">
+        <v>10145</v>
       </c>
       <c r="D21" s="18">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E21" s="18">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="F21" s="5"/>
-      <c r="G21" s="19">
+      <c r="G21" s="20">
         <v>17</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+      <c r="H21" s="20">
+        <v>30</v>
+      </c>
+      <c r="I21" s="21">
+        <v>8290</v>
+      </c>
+      <c r="J21" s="20">
+        <v>114</v>
+      </c>
+      <c r="K21" s="20">
+        <v>110</v>
+      </c>
     </row>
     <row r="22" ht="16" customHeight="1">
       <c r="A22" s="18">
@@ -1937,267 +2085,347 @@
       <c r="B22" s="18">
         <v>12</v>
       </c>
-      <c r="C22" s="18">
-        <v>11185</v>
+      <c r="C22" s="19">
+        <v>10145</v>
       </c>
       <c r="D22" s="18">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="E22" s="18">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="F22" s="5"/>
-      <c r="G22" s="19">
+      <c r="G22" s="20">
         <v>18</v>
       </c>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+      <c r="H22" s="20">
+        <v>30</v>
+      </c>
+      <c r="I22" s="21">
+        <v>8290</v>
+      </c>
+      <c r="J22" s="20">
+        <v>104</v>
+      </c>
+      <c r="K22" s="20">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" ht="16" customHeight="1">
       <c r="A23" s="18">
         <v>19</v>
       </c>
       <c r="B23" s="18">
-        <v>13</v>
-      </c>
-      <c r="C23" s="18">
-        <v>11185</v>
+        <v>12</v>
+      </c>
+      <c r="C23" s="19">
+        <v>11145</v>
       </c>
       <c r="D23" s="18">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E23" s="18">
+        <v>50</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="20">
+        <v>19</v>
+      </c>
+      <c r="H23" s="20">
         <v>30</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="19">
-        <v>19</v>
-      </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+      <c r="I23" s="21">
+        <v>9290</v>
+      </c>
+      <c r="J23" s="20">
+        <v>80</v>
+      </c>
+      <c r="K23" s="20">
+        <v>82</v>
+      </c>
     </row>
     <row r="24" ht="16" customHeight="1">
       <c r="A24" s="18">
         <v>20</v>
       </c>
       <c r="B24" s="18">
-        <v>15</v>
-      </c>
-      <c r="C24" s="18">
-        <v>10405</v>
+        <v>13</v>
+      </c>
+      <c r="C24" s="19">
+        <v>11145</v>
       </c>
       <c r="D24" s="18">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="E24" s="18">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F24" s="5"/>
-      <c r="G24" s="19">
+      <c r="G24" s="20">
         <v>20</v>
       </c>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+      <c r="H24" s="20">
+        <v>30</v>
+      </c>
+      <c r="I24" s="21">
+        <v>10290</v>
+      </c>
+      <c r="J24" s="20">
+        <v>56</v>
+      </c>
+      <c r="K24" s="20">
+        <v>64</v>
+      </c>
     </row>
     <row r="25" ht="16" customHeight="1">
       <c r="A25" s="18">
         <v>21</v>
       </c>
       <c r="B25" s="18">
-        <v>9</v>
-      </c>
-      <c r="C25" s="18">
-        <v>10405</v>
+        <v>15</v>
+      </c>
+      <c r="C25" s="19">
+        <v>10465</v>
       </c>
       <c r="D25" s="18">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E25" s="18">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F25" s="5"/>
-      <c r="G25" s="19">
+      <c r="G25" s="20">
         <v>21</v>
       </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+      <c r="H25" s="20">
+        <v>30</v>
+      </c>
+      <c r="I25" s="21">
+        <v>11290</v>
+      </c>
+      <c r="J25" s="20">
+        <v>41</v>
+      </c>
+      <c r="K25" s="20">
+        <v>43</v>
+      </c>
     </row>
     <row r="26" ht="16" customHeight="1">
       <c r="A26" s="18">
         <v>22</v>
       </c>
       <c r="B26" s="18">
-        <v>21</v>
-      </c>
-      <c r="C26" s="18">
-        <v>10405</v>
+        <v>9</v>
+      </c>
+      <c r="C26" s="19">
+        <v>10465</v>
       </c>
       <c r="D26" s="18">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="E26" s="18">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="19">
+      <c r="G26" s="20">
         <v>22</v>
       </c>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+      <c r="H26" s="20">
+        <v>30</v>
+      </c>
+      <c r="I26" s="21">
+        <v>12290</v>
+      </c>
+      <c r="J26" s="20">
+        <v>26</v>
+      </c>
+      <c r="K26" s="20">
+        <v>22</v>
+      </c>
     </row>
     <row r="27" ht="16" customHeight="1">
       <c r="A27" s="18">
         <v>23</v>
       </c>
       <c r="B27" s="18">
-        <v>27</v>
-      </c>
-      <c r="C27" s="18">
-        <v>10405</v>
+        <v>21</v>
+      </c>
+      <c r="C27" s="19">
+        <v>10465</v>
       </c>
       <c r="D27" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E27" s="18">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F27" s="5"/>
-      <c r="G27" s="19">
+      <c r="G27" s="20">
         <v>23</v>
       </c>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
+      <c r="H27" s="20">
+        <v>39</v>
+      </c>
+      <c r="I27" s="21">
+        <v>11130</v>
+      </c>
+      <c r="J27" s="20">
+        <v>46</v>
+      </c>
+      <c r="K27" s="20">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" ht="16" customHeight="1">
       <c r="A28" s="18">
         <v>24</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="19">
+      <c r="G28" s="20">
         <v>24</v>
       </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
+      <c r="H28" s="20">
+        <v>47</v>
+      </c>
+      <c r="I28" s="21">
+        <v>11130</v>
+      </c>
+      <c r="J28" s="20">
+        <v>36</v>
+      </c>
+      <c r="K28" s="20">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" ht="16" customHeight="1">
       <c r="A29" s="18">
         <v>25</v>
       </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="22"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="19">
+      <c r="G29" s="20">
         <v>25</v>
       </c>
-      <c r="H29" s="20"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
+      <c r="H29" s="20">
+        <v>47</v>
+      </c>
+      <c r="I29" s="21">
+        <v>11130</v>
+      </c>
+      <c r="J29" s="20">
+        <v>26</v>
+      </c>
+      <c r="K29" s="20">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" ht="16" customHeight="1">
       <c r="A30" s="18">
         <v>26</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
       <c r="F30" s="5"/>
-      <c r="G30" s="19">
+      <c r="G30" s="20">
         <v>26</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
+      <c r="H30" s="20">
+        <v>56</v>
+      </c>
+      <c r="I30" s="21">
+        <v>11130</v>
+      </c>
+      <c r="J30" s="20">
+        <v>10</v>
+      </c>
+      <c r="K30" s="20">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" ht="16" customHeight="1">
       <c r="A31" s="18">
         <v>27</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
       <c r="F31" s="5"/>
-      <c r="G31" s="19">
+      <c r="G31" s="20">
         <v>27</v>
       </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
+      <c r="H31" s="20">
+        <v>64</v>
+      </c>
+      <c r="I31" s="21">
+        <v>11130</v>
+      </c>
+      <c r="J31" s="20">
+        <v>0</v>
+      </c>
+      <c r="K31" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="32" ht="16" customHeight="1">
       <c r="A32" s="18">
         <v>28</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="21"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="19">
+      <c r="G32" s="20">
         <v>28</v>
       </c>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
     </row>
     <row r="33" ht="16" customHeight="1">
       <c r="A33" s="18">
         <v>29</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="19">
+      <c r="G33" s="20">
         <v>29</v>
       </c>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
     </row>
     <row r="34" ht="16" customHeight="1">
       <c r="A34" s="18">
         <v>30</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="19">
+      <c r="G34" s="20">
         <v>30</v>
       </c>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final change? I guess?
</commit_message>
<xml_diff>
--- a/data/ans.1.xlsx
+++ b/data/ans.1.xlsx
@@ -256,7 +256,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -317,16 +317,13 @@
     <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1508,13 +1505,13 @@
         <v>1</v>
       </c>
       <c r="I4" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J4" s="20">
-        <v>166</v>
+        <v>247</v>
       </c>
       <c r="K4" s="20">
-        <v>351</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" ht="16" customHeight="1">
@@ -1541,13 +1538,13 @@
         <v>2</v>
       </c>
       <c r="I5" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J5" s="20">
-        <v>150</v>
+        <v>231</v>
       </c>
       <c r="K5" s="20">
-        <v>339</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
@@ -1574,13 +1571,13 @@
         <v>3</v>
       </c>
       <c r="I6" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J6" s="20">
-        <v>134</v>
+        <v>215</v>
       </c>
       <c r="K6" s="20">
-        <v>327</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
@@ -1607,13 +1604,13 @@
         <v>4</v>
       </c>
       <c r="I7" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J7" s="20">
-        <v>124</v>
+        <v>205</v>
       </c>
       <c r="K7" s="20">
-        <v>313</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
@@ -1640,13 +1637,13 @@
         <v>4</v>
       </c>
       <c r="I8" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J8" s="20">
-        <v>114</v>
+        <v>195</v>
       </c>
       <c r="K8" s="20">
-        <v>303</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1">
@@ -1673,13 +1670,13 @@
         <v>5</v>
       </c>
       <c r="I9" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J9" s="20">
-        <v>104</v>
+        <v>185</v>
       </c>
       <c r="K9" s="20">
-        <v>289</v>
+        <v>167</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
@@ -1706,13 +1703,13 @@
         <v>13</v>
       </c>
       <c r="I10" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J10" s="20">
-        <v>88</v>
+        <v>169</v>
       </c>
       <c r="K10" s="20">
-        <v>277</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" ht="16" customHeight="1">
@@ -1739,13 +1736,13 @@
         <v>13</v>
       </c>
       <c r="I11" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J11" s="20">
-        <v>78</v>
+        <v>159</v>
       </c>
       <c r="K11" s="20">
-        <v>267</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" ht="16" customHeight="1">
@@ -1772,13 +1769,13 @@
         <v>22</v>
       </c>
       <c r="I12" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J12" s="20">
-        <v>68</v>
+        <v>149</v>
       </c>
       <c r="K12" s="20">
-        <v>253</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" ht="16" customHeight="1">
@@ -1805,13 +1802,13 @@
         <v>30</v>
       </c>
       <c r="I13" s="21">
-        <v>5660</v>
+        <v>6475</v>
       </c>
       <c r="J13" s="20">
-        <v>52</v>
+        <v>133</v>
       </c>
       <c r="K13" s="20">
-        <v>241</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" ht="16" customHeight="1">
@@ -1835,16 +1832,16 @@
         <v>10</v>
       </c>
       <c r="H14" s="20">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I14" s="21">
-        <v>5660</v>
+        <v>7475</v>
       </c>
       <c r="J14" s="20">
-        <v>36</v>
+        <v>109</v>
       </c>
       <c r="K14" s="20">
-        <v>229</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" ht="16" customHeight="1">
@@ -1868,16 +1865,16 @@
         <v>11</v>
       </c>
       <c r="H15" s="20">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I15" s="21">
-        <v>3290</v>
+        <v>8475</v>
       </c>
       <c r="J15" s="20">
-        <v>247</v>
+        <v>79</v>
       </c>
       <c r="K15" s="20">
-        <v>227</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" ht="16" customHeight="1">
@@ -1904,13 +1901,13 @@
         <v>30</v>
       </c>
       <c r="I16" s="21">
-        <v>3290</v>
+        <v>9475</v>
       </c>
       <c r="J16" s="20">
-        <v>231</v>
+        <v>55</v>
       </c>
       <c r="K16" s="20">
-        <v>215</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" ht="16" customHeight="1">
@@ -1937,13 +1934,13 @@
         <v>30</v>
       </c>
       <c r="I17" s="21">
-        <v>4290</v>
+        <v>10475</v>
       </c>
       <c r="J17" s="20">
-        <v>216</v>
+        <v>40</v>
       </c>
       <c r="K17" s="20">
-        <v>194</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" ht="16" customHeight="1">
@@ -1970,13 +1967,13 @@
         <v>30</v>
       </c>
       <c r="I18" s="21">
-        <v>5290</v>
+        <v>11475</v>
       </c>
       <c r="J18" s="20">
-        <v>192</v>
+        <v>16</v>
       </c>
       <c r="K18" s="20">
-        <v>176</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" ht="16" customHeight="1">
@@ -2000,16 +1997,16 @@
         <v>15</v>
       </c>
       <c r="H19" s="20">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="I19" s="21">
-        <v>6290</v>
+        <v>4525</v>
       </c>
       <c r="J19" s="20">
-        <v>168</v>
+        <v>237</v>
       </c>
       <c r="K19" s="20">
-        <v>158</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" ht="16" customHeight="1">
@@ -2036,13 +2033,13 @@
         <v>30</v>
       </c>
       <c r="I20" s="21">
-        <v>7290</v>
+        <v>4525</v>
       </c>
       <c r="J20" s="20">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="K20" s="20">
-        <v>140</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" ht="16" customHeight="1">
@@ -2069,13 +2066,13 @@
         <v>30</v>
       </c>
       <c r="I21" s="21">
-        <v>8290</v>
+        <v>4525</v>
       </c>
       <c r="J21" s="20">
-        <v>114</v>
+        <v>211</v>
       </c>
       <c r="K21" s="20">
-        <v>110</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" ht="16" customHeight="1">
@@ -2102,13 +2099,13 @@
         <v>30</v>
       </c>
       <c r="I22" s="21">
-        <v>8290</v>
+        <v>5525</v>
       </c>
       <c r="J22" s="20">
-        <v>104</v>
+        <v>181</v>
       </c>
       <c r="K22" s="20">
-        <v>100</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" ht="16" customHeight="1">
@@ -2135,13 +2132,13 @@
         <v>30</v>
       </c>
       <c r="I23" s="21">
-        <v>9290</v>
+        <v>6525</v>
       </c>
       <c r="J23" s="20">
-        <v>80</v>
+        <v>157</v>
       </c>
       <c r="K23" s="20">
-        <v>82</v>
+        <v>161</v>
       </c>
     </row>
     <row r="24" ht="16" customHeight="1">
@@ -2168,13 +2165,13 @@
         <v>30</v>
       </c>
       <c r="I24" s="21">
-        <v>10290</v>
+        <v>7525</v>
       </c>
       <c r="J24" s="20">
-        <v>56</v>
+        <v>133</v>
       </c>
       <c r="K24" s="20">
-        <v>64</v>
+        <v>143</v>
       </c>
     </row>
     <row r="25" ht="16" customHeight="1">
@@ -2201,13 +2198,13 @@
         <v>30</v>
       </c>
       <c r="I25" s="21">
-        <v>11290</v>
+        <v>8525</v>
       </c>
       <c r="J25" s="20">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="K25" s="20">
-        <v>43</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" ht="16" customHeight="1">
@@ -2234,13 +2231,13 @@
         <v>30</v>
       </c>
       <c r="I26" s="21">
-        <v>12290</v>
+        <v>9525</v>
       </c>
       <c r="J26" s="20">
-        <v>26</v>
+        <v>103</v>
       </c>
       <c r="K26" s="20">
-        <v>22</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" ht="16" customHeight="1">
@@ -2264,16 +2261,16 @@
         <v>23</v>
       </c>
       <c r="H27" s="20">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I27" s="21">
-        <v>11130</v>
+        <v>10525</v>
       </c>
       <c r="J27" s="20">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="K27" s="20">
-        <v>50</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" ht="16" customHeight="1">
@@ -2289,16 +2286,16 @@
         <v>24</v>
       </c>
       <c r="H28" s="20">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="I28" s="21">
-        <v>11130</v>
+        <v>11525</v>
       </c>
       <c r="J28" s="20">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="K28" s="20">
-        <v>36</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" ht="16" customHeight="1">
@@ -2314,16 +2311,16 @@
         <v>25</v>
       </c>
       <c r="H29" s="20">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="I29" s="21">
-        <v>11130</v>
+        <v>12525</v>
       </c>
       <c r="J29" s="20">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K29" s="20">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" ht="16" customHeight="1">
@@ -2339,10 +2336,10 @@
         <v>26</v>
       </c>
       <c r="H30" s="20">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="I30" s="21">
-        <v>11130</v>
+        <v>13525</v>
       </c>
       <c r="J30" s="20">
         <v>10</v>
@@ -2364,16 +2361,16 @@
         <v>27</v>
       </c>
       <c r="H31" s="20">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="I31" s="21">
-        <v>11130</v>
+        <v>12345</v>
       </c>
       <c r="J31" s="20">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="K31" s="20">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" ht="16" customHeight="1">
@@ -2388,10 +2385,18 @@
       <c r="G32" s="20">
         <v>28</v>
       </c>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
+      <c r="H32" s="20">
+        <v>47</v>
+      </c>
+      <c r="I32" s="21">
+        <v>12345</v>
+      </c>
+      <c r="J32" s="20">
+        <v>32</v>
+      </c>
+      <c r="K32" s="20">
+        <v>24</v>
+      </c>
     </row>
     <row r="33" ht="16" customHeight="1">
       <c r="A33" s="18">
@@ -2405,10 +2410,18 @@
       <c r="G33" s="20">
         <v>29</v>
       </c>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-      <c r="K33" s="23"/>
+      <c r="H33" s="20">
+        <v>56</v>
+      </c>
+      <c r="I33" s="21">
+        <v>12345</v>
+      </c>
+      <c r="J33" s="20">
+        <v>16</v>
+      </c>
+      <c r="K33" s="20">
+        <v>12</v>
+      </c>
     </row>
     <row r="34" ht="16" customHeight="1">
       <c r="A34" s="18">
@@ -2422,10 +2435,18 @@
       <c r="G34" s="20">
         <v>30</v>
       </c>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-      <c r="K34" s="23"/>
+      <c r="H34" s="20">
+        <v>64</v>
+      </c>
+      <c r="I34" s="20">
+        <v>12345</v>
+      </c>
+      <c r="J34" s="20">
+        <v>0</v>
+      </c>
+      <c r="K34" s="20">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>